<commit_message>
Use rxridge With STATA 18
</commit_message>
<xml_diff>
--- a/rxridge/rxridge.xlsx
+++ b/rxridge/rxridge.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="19815" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="Regression Panel Data In R Olah" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -29,7 +31,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,334 +40,16 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -373,204 +57,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -865,7 +360,7 @@
   <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2043,4 +1538,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>